<commit_message>
Code completo de analisis de proyeto final
</commit_message>
<xml_diff>
--- a/Docs/Datos filtrados, sin babosadas.xlsx
+++ b/Docs/Datos filtrados, sin babosadas.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Icesi\Semestre5\Inferencia\Proyecto Final\Infrencia\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C6440F-ECE0-4AA2-B01A-A9CD74AEAEE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01661E8-2724-4FFB-95CE-A74421B4720B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Respuestas" sheetId="1" r:id="rId1"/>
-    <sheet name="Preguntas" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="3" r:id="rId2"/>
+    <sheet name="Preguntas" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="38">
   <si>
     <t xml:space="preserve">¿Cual es su sexo? </t>
   </si>
@@ -132,10 +133,22 @@
     <t>data_acoso_result</t>
   </si>
   <si>
+    <t>Hombress</t>
+  </si>
+  <si>
+    <t>Mujeress</t>
+  </si>
+  <si>
     <t>Pregunta 1.1</t>
   </si>
   <si>
     <t>Pregunta 4.4</t>
+  </si>
+  <si>
+    <t>Hombres</t>
+  </si>
+  <si>
+    <t>Mujeres</t>
   </si>
 </sst>
 </file>
@@ -197,7 +210,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -231,11 +244,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -243,18 +282,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="2">
     <dxf>
       <font>
         <b val="0"/>
@@ -269,6 +309,7 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -292,45 +333,9 @@
         <sz val="10"/>
         <color theme="1"/>
         <name val="Arial"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -346,17 +351,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{ED35D98B-CDE8-40BF-884A-D062829D3E20}" name="Tabla3" displayName="Tabla3" ref="U1:V97" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
-  <autoFilter ref="U1:V97" xr:uid="{ED35D98B-CDE8-40BF-884A-D062829D3E20}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Mujer"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6A419242-CB0F-44BD-B2EE-7C86C5AECB60}" name="Tabla1" displayName="Tabla1" ref="X1:Y97" totalsRowShown="0">
+  <autoFilter ref="X1:Y97" xr:uid="{6A419242-CB0F-44BD-B2EE-7C86C5AECB60}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{A899BC29-8580-4B2C-B4F4-5652078ACF03}" name="Pregunta 1.1" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{5C470823-FB93-48DF-9591-97540A0E0741}" name="Pregunta 4.4" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{CCABA226-20C6-43C7-BAE0-8A6AB53395AA}" name="Pregunta 1.1" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{84BCDF1A-0394-48B4-8813-AEBA025B7382}" name="Pregunta 4.4" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -563,11 +562,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD97"/>
+  <dimension ref="A1:AL97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V1" sqref="V1"/>
+    <sheetView topLeftCell="Z1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -581,8 +580,8 @@
     <col min="14" max="17" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>16</v>
       </c>
       <c r="B1" t="s">
@@ -630,15 +629,26 @@
       <c r="R1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="U1" s="13" t="s">
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="X1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+      <c r="AD1" s="7"/>
+      <c r="AJ1" t="s">
         <v>32</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="AL1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -686,21 +696,28 @@
       <c r="R2">
         <v>1</v>
       </c>
-      <c r="U2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V2" s="6">
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="X2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y2" s="6">
         <v>2</v>
       </c>
-      <c r="Z2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA2" s="9">
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="9"/>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="9"/>
+      <c r="AG2" s="12"/>
+      <c r="AJ2" s="11">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:30" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="AL2" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -748,21 +765,28 @@
       <c r="R3">
         <v>0</v>
       </c>
-      <c r="U3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V3" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA3" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="X3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y3" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="9"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="9"/>
+      <c r="AG3" s="12"/>
+      <c r="AJ3" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -810,21 +834,28 @@
       <c r="R4">
         <v>0</v>
       </c>
-      <c r="U4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V4" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA4" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="X4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y4" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="9"/>
+      <c r="AC4" s="8"/>
+      <c r="AD4" s="9"/>
+      <c r="AG4" s="12"/>
+      <c r="AJ4" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -872,21 +903,28 @@
       <c r="R5">
         <v>1</v>
       </c>
-      <c r="U5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V5" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA5" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="X5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y5" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="9"/>
+      <c r="AC5" s="8"/>
+      <c r="AD5" s="9"/>
+      <c r="AG5" s="12"/>
+      <c r="AJ5" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL5" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -934,21 +972,28 @@
       <c r="R6">
         <v>1</v>
       </c>
-      <c r="U6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V6" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA6" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="X6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y6" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="8"/>
+      <c r="AA6" s="9"/>
+      <c r="AC6" s="8"/>
+      <c r="AD6" s="9"/>
+      <c r="AG6" s="12"/>
+      <c r="AJ6" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -996,27 +1041,28 @@
       <c r="R7">
         <v>1</v>
       </c>
-      <c r="U7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V7" s="6">
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="X7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y7" s="6">
         <v>2</v>
       </c>
-      <c r="Z7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA7" s="9">
+      <c r="Z7" s="8"/>
+      <c r="AA7" s="9"/>
+      <c r="AC7" s="8"/>
+      <c r="AD7" s="9"/>
+      <c r="AG7" s="12"/>
+      <c r="AJ7" s="11">
         <v>2</v>
       </c>
-      <c r="AC7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD7" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="AL7" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1064,27 +1110,28 @@
       <c r="R8">
         <v>1</v>
       </c>
-      <c r="U8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V8" s="6">
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="X8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y8" s="6">
         <v>2</v>
       </c>
-      <c r="Z8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA8" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD8" s="9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="Z8" s="8"/>
+      <c r="AA8" s="9"/>
+      <c r="AC8" s="8"/>
+      <c r="AD8" s="9"/>
+      <c r="AG8" s="12"/>
+      <c r="AJ8" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL8" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1132,27 +1179,28 @@
       <c r="R9">
         <v>0</v>
       </c>
-      <c r="U9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V9" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA9" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD9" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="X9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y9" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="8"/>
+      <c r="AA9" s="9"/>
+      <c r="AC9" s="8"/>
+      <c r="AD9" s="9"/>
+      <c r="AG9" s="12"/>
+      <c r="AJ9" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL9" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1200,27 +1248,28 @@
       <c r="R10">
         <v>0</v>
       </c>
-      <c r="U10" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V10" s="6">
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="X10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y10" s="6">
         <v>5</v>
       </c>
-      <c r="Z10" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA10" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD10" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="Z10" s="8"/>
+      <c r="AA10" s="9"/>
+      <c r="AC10" s="8"/>
+      <c r="AD10" s="9"/>
+      <c r="AG10" s="12"/>
+      <c r="AJ10" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL10" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1268,27 +1317,28 @@
       <c r="R11">
         <v>1</v>
       </c>
-      <c r="U11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V11" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA11" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC11" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD11" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:30" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="X11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y11" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="8"/>
+      <c r="AA11" s="9"/>
+      <c r="AC11" s="8"/>
+      <c r="AD11" s="9"/>
+      <c r="AG11" s="12"/>
+      <c r="AJ11" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL11" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1336,27 +1386,28 @@
       <c r="R12">
         <v>0</v>
       </c>
-      <c r="U12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V12" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA12" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC12" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD12" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="X12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y12" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="8"/>
+      <c r="AA12" s="9"/>
+      <c r="AC12" s="8"/>
+      <c r="AD12" s="9"/>
+      <c r="AG12" s="12"/>
+      <c r="AJ12" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL12" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1404,27 +1455,28 @@
       <c r="R13">
         <v>0</v>
       </c>
-      <c r="U13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V13" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA13" s="9">
-        <v>1</v>
-      </c>
-      <c r="AC13" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD13" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="X13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y13" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="8"/>
+      <c r="AA13" s="9"/>
+      <c r="AC13" s="8"/>
+      <c r="AD13" s="9"/>
+      <c r="AG13" s="12"/>
+      <c r="AJ13" s="11">
+        <v>1</v>
+      </c>
+      <c r="AL13" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1472,27 +1524,28 @@
       <c r="R14">
         <v>1</v>
       </c>
-      <c r="U14" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V14" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA14" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC14" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD14" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="X14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y14" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="8"/>
+      <c r="AA14" s="9"/>
+      <c r="AC14" s="8"/>
+      <c r="AD14" s="9"/>
+      <c r="AG14" s="12"/>
+      <c r="AJ14" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL14" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -1540,27 +1593,28 @@
       <c r="R15">
         <v>0</v>
       </c>
-      <c r="U15" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V15" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z15" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA15" s="9">
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="X15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y15" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="8"/>
+      <c r="AA15" s="9"/>
+      <c r="AC15" s="8"/>
+      <c r="AD15" s="9"/>
+      <c r="AG15" s="12"/>
+      <c r="AJ15" s="11">
         <v>2</v>
       </c>
-      <c r="AC15" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD15" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="AL15" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1608,27 +1662,28 @@
       <c r="R16">
         <v>0</v>
       </c>
-      <c r="U16" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V16" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z16" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA16" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC16" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD16" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="X16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y16" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="8"/>
+      <c r="AA16" s="9"/>
+      <c r="AC16" s="8"/>
+      <c r="AD16" s="9"/>
+      <c r="AG16" s="12"/>
+      <c r="AJ16" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL16" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1676,27 +1731,28 @@
       <c r="R17">
         <v>1</v>
       </c>
-      <c r="U17" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V17" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA17" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC17" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD17" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="X17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y17" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="8"/>
+      <c r="AA17" s="9"/>
+      <c r="AC17" s="8"/>
+      <c r="AD17" s="9"/>
+      <c r="AG17" s="12"/>
+      <c r="AJ17" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL17" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1744,27 +1800,28 @@
       <c r="R18">
         <v>1</v>
       </c>
-      <c r="U18" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V18" s="6">
-        <v>1</v>
-      </c>
-      <c r="Z18" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA18" s="9">
-        <v>1</v>
-      </c>
-      <c r="AC18" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD18" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:30" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="X18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y18" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z18" s="8"/>
+      <c r="AA18" s="9"/>
+      <c r="AC18" s="8"/>
+      <c r="AD18" s="9"/>
+      <c r="AG18" s="12"/>
+      <c r="AJ18" s="11">
+        <v>1</v>
+      </c>
+      <c r="AL18" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1812,27 +1869,28 @@
       <c r="R19">
         <v>1</v>
       </c>
-      <c r="U19" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V19" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z19" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA19" s="9">
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="X19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y19" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="8"/>
+      <c r="AA19" s="9"/>
+      <c r="AC19" s="8"/>
+      <c r="AD19" s="9"/>
+      <c r="AG19" s="12"/>
+      <c r="AJ19" s="11">
         <v>5</v>
       </c>
-      <c r="AC19" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD19" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="AL19" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1880,27 +1938,28 @@
       <c r="R20">
         <v>1</v>
       </c>
-      <c r="U20" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V20" s="6">
-        <v>1</v>
-      </c>
-      <c r="Z20" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA20" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC20" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD20" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="X20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y20" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z20" s="8"/>
+      <c r="AA20" s="9"/>
+      <c r="AC20" s="8"/>
+      <c r="AD20" s="9"/>
+      <c r="AG20" s="12"/>
+      <c r="AJ20" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL20" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1948,27 +2007,28 @@
       <c r="R21">
         <v>1</v>
       </c>
-      <c r="U21" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V21" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z21" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA21" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC21" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD21" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:30" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="X21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y21" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="8"/>
+      <c r="AA21" s="9"/>
+      <c r="AC21" s="8"/>
+      <c r="AD21" s="9"/>
+      <c r="AG21" s="12"/>
+      <c r="AJ21" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL21" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -2016,27 +2076,28 @@
       <c r="R22">
         <v>1</v>
       </c>
-      <c r="U22" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V22" s="6">
-        <v>1</v>
-      </c>
-      <c r="Z22" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA22" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC22" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD22" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:30" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="X22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y22" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z22" s="8"/>
+      <c r="AA22" s="9"/>
+      <c r="AC22" s="8"/>
+      <c r="AD22" s="9"/>
+      <c r="AG22" s="12"/>
+      <c r="AJ22" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL22" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -2084,27 +2145,28 @@
       <c r="R23">
         <v>0</v>
       </c>
-      <c r="U23" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V23" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z23" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA23" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC23" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD23" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:30" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="X23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y23" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="8"/>
+      <c r="AA23" s="9"/>
+      <c r="AC23" s="8"/>
+      <c r="AD23" s="9"/>
+      <c r="AG23" s="12"/>
+      <c r="AJ23" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL23" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -2152,27 +2214,28 @@
       <c r="R24">
         <v>1</v>
       </c>
-      <c r="U24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V24" s="6">
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="X24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y24" s="6">
         <v>2</v>
       </c>
-      <c r="Z24" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA24" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC24" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD24" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+      <c r="Z24" s="8"/>
+      <c r="AA24" s="9"/>
+      <c r="AC24" s="8"/>
+      <c r="AD24" s="9"/>
+      <c r="AG24" s="12"/>
+      <c r="AJ24" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL24" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -2220,27 +2283,28 @@
       <c r="R25">
         <v>1</v>
       </c>
-      <c r="U25" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V25" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z25" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA25" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC25" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD25" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:30" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="X25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y25" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="8"/>
+      <c r="AA25" s="9"/>
+      <c r="AC25" s="8"/>
+      <c r="AD25" s="9"/>
+      <c r="AG25" s="12"/>
+      <c r="AJ25" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL25" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -2288,27 +2352,28 @@
       <c r="R26">
         <v>1</v>
       </c>
-      <c r="U26" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V26" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z26" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA26" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC26" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD26" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="X26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y26" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="8"/>
+      <c r="AA26" s="9"/>
+      <c r="AC26" s="8"/>
+      <c r="AD26" s="9"/>
+      <c r="AG26" s="12"/>
+      <c r="AJ26" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL26" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -2356,27 +2421,28 @@
       <c r="R27">
         <v>1</v>
       </c>
-      <c r="U27" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V27" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z27" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA27" s="9">
-        <v>1</v>
-      </c>
-      <c r="AC27" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD27" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="X27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y27" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="8"/>
+      <c r="AA27" s="9"/>
+      <c r="AC27" s="8"/>
+      <c r="AD27" s="9"/>
+      <c r="AG27" s="12"/>
+      <c r="AJ27" s="11">
+        <v>1</v>
+      </c>
+      <c r="AL27" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -2424,27 +2490,28 @@
       <c r="R28">
         <v>1</v>
       </c>
-      <c r="U28" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V28" s="6">
-        <v>1</v>
-      </c>
-      <c r="Z28" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA28" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC28" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD28" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:30" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="X28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y28" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z28" s="8"/>
+      <c r="AA28" s="9"/>
+      <c r="AC28" s="8"/>
+      <c r="AD28" s="9"/>
+      <c r="AG28" s="12"/>
+      <c r="AJ28" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL28" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -2492,27 +2559,28 @@
       <c r="R29">
         <v>0</v>
       </c>
-      <c r="U29" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V29" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z29" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA29" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC29" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD29" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:30" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="X29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y29" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z29" s="8"/>
+      <c r="AA29" s="9"/>
+      <c r="AC29" s="8"/>
+      <c r="AD29" s="9"/>
+      <c r="AG29" s="12"/>
+      <c r="AJ29" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL29" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -2560,27 +2628,28 @@
       <c r="R30">
         <v>1</v>
       </c>
-      <c r="U30" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V30" s="6">
-        <v>1</v>
-      </c>
-      <c r="Z30" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA30" s="9">
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="X30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y30" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z30" s="8"/>
+      <c r="AA30" s="9"/>
+      <c r="AC30" s="8"/>
+      <c r="AD30" s="9"/>
+      <c r="AG30" s="12"/>
+      <c r="AJ30" s="11">
         <v>3</v>
       </c>
-      <c r="AC30" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD30" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
+      <c r="AL30" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B31" s="1" t="s">
@@ -2628,27 +2697,28 @@
       <c r="R31">
         <v>0</v>
       </c>
-      <c r="U31" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V31" s="6">
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="X31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y31" s="6">
         <v>3</v>
       </c>
-      <c r="Z31" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA31" s="9">
-        <v>1</v>
-      </c>
-      <c r="AC31" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD31" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
+      <c r="Z31" s="8"/>
+      <c r="AA31" s="9"/>
+      <c r="AC31" s="8"/>
+      <c r="AD31" s="9"/>
+      <c r="AG31" s="12"/>
+      <c r="AJ31" s="11">
+        <v>1</v>
+      </c>
+      <c r="AL31" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -2696,27 +2766,28 @@
       <c r="R32">
         <v>1</v>
       </c>
-      <c r="U32" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V32" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z32" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA32" s="9">
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="X32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y32" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z32" s="8"/>
+      <c r="AA32" s="9"/>
+      <c r="AC32" s="8"/>
+      <c r="AD32" s="9"/>
+      <c r="AG32" s="12"/>
+      <c r="AJ32" s="11">
         <v>2</v>
       </c>
-      <c r="AC32" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD32" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A33" s="11" t="s">
+      <c r="AL32" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -2764,27 +2835,28 @@
       <c r="R33">
         <v>0</v>
       </c>
-      <c r="U33" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V33" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z33" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA33" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC33" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD33" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:30" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="11" t="s">
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="X33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y33" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z33" s="8"/>
+      <c r="AA33" s="9"/>
+      <c r="AC33" s="8"/>
+      <c r="AD33" s="9"/>
+      <c r="AG33" s="12"/>
+      <c r="AJ33" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL33" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B34" s="1" t="s">
@@ -2832,27 +2904,28 @@
       <c r="R34">
         <v>1</v>
       </c>
-      <c r="U34" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V34" s="6">
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+      <c r="X34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y34" s="6">
         <v>5</v>
       </c>
-      <c r="Z34" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA34" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC34" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD34" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A35" s="11" t="s">
+      <c r="Z34" s="8"/>
+      <c r="AA34" s="9"/>
+      <c r="AC34" s="8"/>
+      <c r="AD34" s="9"/>
+      <c r="AG34" s="12"/>
+      <c r="AJ34" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL34" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -2900,27 +2973,28 @@
       <c r="R35">
         <v>0</v>
       </c>
-      <c r="U35" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V35" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z35" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA35" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC35" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD35" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:30" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="11" t="s">
+      <c r="U35" s="1"/>
+      <c r="V35" s="1"/>
+      <c r="X35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y35" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z35" s="8"/>
+      <c r="AA35" s="9"/>
+      <c r="AC35" s="8"/>
+      <c r="AD35" s="9"/>
+      <c r="AG35" s="12"/>
+      <c r="AJ35" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL35" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -2968,27 +3042,28 @@
       <c r="R36">
         <v>1</v>
       </c>
-      <c r="U36" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V36" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z36" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA36" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC36" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD36" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
+      <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
+      <c r="X36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y36" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z36" s="8"/>
+      <c r="AA36" s="9"/>
+      <c r="AC36" s="8"/>
+      <c r="AD36" s="9"/>
+      <c r="AG36" s="12"/>
+      <c r="AJ36" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL36" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -3036,27 +3111,28 @@
       <c r="R37">
         <v>0</v>
       </c>
-      <c r="U37" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V37" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z37" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA37" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC37" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD37" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
+      <c r="U37" s="1"/>
+      <c r="V37" s="1"/>
+      <c r="X37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y37" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z37" s="8"/>
+      <c r="AA37" s="9"/>
+      <c r="AC37" s="8"/>
+      <c r="AD37" s="9"/>
+      <c r="AG37" s="12"/>
+      <c r="AJ37" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL37" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -3104,27 +3180,28 @@
       <c r="R38">
         <v>0</v>
       </c>
-      <c r="U38" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V38" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z38" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA38" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC38" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD38" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:30" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
+      <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
+      <c r="X38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y38" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z38" s="8"/>
+      <c r="AA38" s="9"/>
+      <c r="AC38" s="8"/>
+      <c r="AD38" s="9"/>
+      <c r="AG38" s="12"/>
+      <c r="AJ38" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL38" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -3172,27 +3249,28 @@
       <c r="R39">
         <v>0</v>
       </c>
-      <c r="U39" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V39" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z39" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA39" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC39" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD39" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A40" s="11" t="s">
+      <c r="U39" s="1"/>
+      <c r="V39" s="1"/>
+      <c r="X39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y39" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z39" s="8"/>
+      <c r="AA39" s="9"/>
+      <c r="AC39" s="8"/>
+      <c r="AD39" s="9"/>
+      <c r="AG39" s="12"/>
+      <c r="AJ39" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL39" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -3240,27 +3318,28 @@
       <c r="R40">
         <v>0</v>
       </c>
-      <c r="U40" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V40" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z40" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA40" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC40" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD40" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:30" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
+      <c r="U40" s="1"/>
+      <c r="V40" s="1"/>
+      <c r="X40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y40" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z40" s="8"/>
+      <c r="AA40" s="9"/>
+      <c r="AC40" s="8"/>
+      <c r="AD40" s="9"/>
+      <c r="AG40" s="12"/>
+      <c r="AJ40" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL40" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -3308,27 +3387,28 @@
       <c r="R41">
         <v>0</v>
       </c>
-      <c r="U41" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V41" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z41" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA41" s="9">
-        <v>1</v>
-      </c>
-      <c r="AC41" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD41" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:30" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="11" t="s">
+      <c r="U41" s="1"/>
+      <c r="V41" s="1"/>
+      <c r="X41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y41" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z41" s="8"/>
+      <c r="AA41" s="9"/>
+      <c r="AC41" s="8"/>
+      <c r="AD41" s="9"/>
+      <c r="AG41" s="12"/>
+      <c r="AJ41" s="11">
+        <v>1</v>
+      </c>
+      <c r="AL41" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -3376,27 +3456,28 @@
       <c r="R42">
         <v>0</v>
       </c>
-      <c r="U42" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V42" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z42" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA42" s="9">
-        <v>0</v>
-      </c>
-      <c r="AC42" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD42" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A43" s="12" t="s">
+      <c r="U42" s="1"/>
+      <c r="V42" s="1"/>
+      <c r="X42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y42" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z42" s="8"/>
+      <c r="AA42" s="9"/>
+      <c r="AC42" s="8"/>
+      <c r="AD42" s="9"/>
+      <c r="AG42" s="12"/>
+      <c r="AJ42" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL42" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -3444,21 +3525,27 @@
       <c r="R43">
         <v>0</v>
       </c>
-      <c r="U43" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="V43" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z43" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA43" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:30" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="11" t="s">
+      <c r="U43" s="2"/>
+      <c r="V43" s="1"/>
+      <c r="X43" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y43" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z43" s="8"/>
+      <c r="AA43" s="9"/>
+      <c r="AD43" s="7"/>
+      <c r="AG43" s="12"/>
+      <c r="AJ43" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL43" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -3506,21 +3593,26 @@
       <c r="R44">
         <v>1</v>
       </c>
-      <c r="U44" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V44" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z44" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA44" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:30" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
+      <c r="U44" s="1"/>
+      <c r="V44" s="1"/>
+      <c r="X44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y44" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z44" s="8"/>
+      <c r="AA44" s="9"/>
+      <c r="AG44" s="12"/>
+      <c r="AJ44" s="11">
+        <v>1</v>
+      </c>
+      <c r="AL44" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -3568,21 +3660,26 @@
       <c r="R45">
         <v>0</v>
       </c>
-      <c r="U45" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V45" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z45" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA45" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
+      <c r="U45" s="1"/>
+      <c r="V45" s="1"/>
+      <c r="X45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y45" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z45" s="8"/>
+      <c r="AA45" s="9"/>
+      <c r="AG45" s="12"/>
+      <c r="AJ45" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL45" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -3630,21 +3727,26 @@
       <c r="R46">
         <v>0</v>
       </c>
-      <c r="U46" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V46" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z46" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA46" s="9">
+      <c r="U46" s="1"/>
+      <c r="V46" s="1"/>
+      <c r="X46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y46" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z46" s="8"/>
+      <c r="AA46" s="9"/>
+      <c r="AG46" s="12"/>
+      <c r="AJ46" s="11">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:30" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
+      <c r="AL46" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -3692,21 +3794,26 @@
       <c r="R47">
         <v>0</v>
       </c>
-      <c r="U47" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V47" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z47" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA47" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A48" s="12" t="s">
+      <c r="U47" s="1"/>
+      <c r="V47" s="1"/>
+      <c r="X47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y47" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z47" s="8"/>
+      <c r="AA47" s="9"/>
+      <c r="AG47" s="12"/>
+      <c r="AJ47" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL47" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -3754,21 +3861,26 @@
       <c r="R48">
         <v>1</v>
       </c>
-      <c r="U48" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="V48" s="6">
+      <c r="U48" s="2"/>
+      <c r="V48" s="1"/>
+      <c r="X48" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y48" s="6">
         <v>2</v>
       </c>
-      <c r="Z48" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA48" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:27" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="11" t="s">
+      <c r="Z48" s="8"/>
+      <c r="AA48" s="9"/>
+      <c r="AG48" s="12"/>
+      <c r="AJ48" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL48" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -3816,21 +3928,26 @@
       <c r="R49">
         <v>1</v>
       </c>
-      <c r="U49" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V49" s="6">
-        <v>1</v>
-      </c>
-      <c r="Z49" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA49" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A50" s="11" t="s">
+      <c r="U49" s="1"/>
+      <c r="V49" s="1"/>
+      <c r="X49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y49" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z49" s="8"/>
+      <c r="AA49" s="9"/>
+      <c r="AG49" s="12"/>
+      <c r="AJ49" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL49" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -3878,21 +3995,26 @@
       <c r="R50">
         <v>0</v>
       </c>
-      <c r="U50" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V50" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z50" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA50" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:27" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
+      <c r="U50" s="1"/>
+      <c r="V50" s="1"/>
+      <c r="X50" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y50" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z50" s="8"/>
+      <c r="AA50" s="9"/>
+      <c r="AG50" s="12"/>
+      <c r="AJ50" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL50" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B51" s="1" t="s">
@@ -3940,21 +4062,26 @@
       <c r="R51">
         <v>1</v>
       </c>
-      <c r="U51" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V51" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z51" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA51" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A52" s="11" t="s">
+      <c r="U51" s="1"/>
+      <c r="V51" s="1"/>
+      <c r="X51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y51" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z51" s="8"/>
+      <c r="AA51" s="9"/>
+      <c r="AG51" s="12"/>
+      <c r="AJ51" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL51" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B52" s="1" t="s">
@@ -4002,21 +4129,26 @@
       <c r="R52">
         <v>1</v>
       </c>
-      <c r="U52" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V52" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z52" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA52" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:27" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="11" t="s">
+      <c r="U52" s="1"/>
+      <c r="V52" s="1"/>
+      <c r="X52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y52" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z52" s="8"/>
+      <c r="AA52" s="9"/>
+      <c r="AG52" s="12"/>
+      <c r="AJ52" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL52" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B53" s="1" t="s">
@@ -4064,21 +4196,26 @@
       <c r="R53">
         <v>0</v>
       </c>
-      <c r="U53" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V53" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z53" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA53" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:27" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="11" t="s">
+      <c r="U53" s="1"/>
+      <c r="V53" s="1"/>
+      <c r="X53" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y53" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z53" s="8"/>
+      <c r="AA53" s="9"/>
+      <c r="AG53" s="12"/>
+      <c r="AJ53" s="11">
+        <v>1</v>
+      </c>
+      <c r="AL53" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B54" s="1" t="s">
@@ -4126,21 +4263,26 @@
       <c r="R54">
         <v>0</v>
       </c>
-      <c r="U54" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V54" s="6">
+      <c r="U54" s="1"/>
+      <c r="V54" s="1"/>
+      <c r="X54" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y54" s="6">
         <v>3</v>
       </c>
-      <c r="Z54" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA54" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:27" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="11" t="s">
+      <c r="Z54" s="8"/>
+      <c r="AA54" s="9"/>
+      <c r="AG54" s="12"/>
+      <c r="AJ54" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL54" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B55" s="1" t="s">
@@ -4188,21 +4330,26 @@
       <c r="R55">
         <v>1</v>
       </c>
-      <c r="U55" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V55" s="6">
-        <v>1</v>
-      </c>
-      <c r="Z55" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA55" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:27" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A56" s="11" t="s">
+      <c r="U55" s="1"/>
+      <c r="V55" s="1"/>
+      <c r="X55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y55" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z55" s="8"/>
+      <c r="AA55" s="9"/>
+      <c r="AG55" s="12"/>
+      <c r="AJ55" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL55" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -4250,21 +4397,26 @@
       <c r="R56">
         <v>1</v>
       </c>
-      <c r="U56" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V56" s="6">
-        <v>1</v>
-      </c>
-      <c r="Z56" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA56" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:27" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="11" t="s">
+      <c r="U56" s="1"/>
+      <c r="V56" s="1"/>
+      <c r="X56" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y56" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z56" s="8"/>
+      <c r="AA56" s="9"/>
+      <c r="AG56" s="12"/>
+      <c r="AJ56" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL56" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -4312,21 +4464,26 @@
       <c r="R57">
         <v>1</v>
       </c>
-      <c r="U57" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V57" s="6">
+      <c r="U57" s="1"/>
+      <c r="V57" s="1"/>
+      <c r="X57" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y57" s="6">
         <v>2</v>
       </c>
-      <c r="Z57" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA57" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:27" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="11" t="s">
+      <c r="Z57" s="8"/>
+      <c r="AA57" s="9"/>
+      <c r="AG57" s="12"/>
+      <c r="AJ57" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL57" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -4374,21 +4531,26 @@
       <c r="R58">
         <v>0</v>
       </c>
-      <c r="U58" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V58" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z58" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA58" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:27" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="11" t="s">
+      <c r="U58" s="1"/>
+      <c r="V58" s="1"/>
+      <c r="X58" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y58" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z58" s="8"/>
+      <c r="AA58" s="9"/>
+      <c r="AG58" s="12"/>
+      <c r="AJ58" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL58" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -4436,21 +4598,26 @@
       <c r="R59">
         <v>0</v>
       </c>
-      <c r="U59" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V59" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z59" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA59" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:27" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="11" t="s">
+      <c r="U59" s="1"/>
+      <c r="V59" s="1"/>
+      <c r="X59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y59" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z59" s="8"/>
+      <c r="AA59" s="9"/>
+      <c r="AG59" s="12"/>
+      <c r="AJ59" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL59" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -4498,21 +4665,26 @@
       <c r="R60">
         <v>0</v>
       </c>
-      <c r="U60" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V60" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z60" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA60" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:27" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="11" t="s">
+      <c r="U60" s="1"/>
+      <c r="V60" s="1"/>
+      <c r="X60" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y60" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z60" s="8"/>
+      <c r="AA60" s="9"/>
+      <c r="AG60" s="12"/>
+      <c r="AJ60" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL60" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -4560,21 +4732,26 @@
       <c r="R61">
         <v>0</v>
       </c>
-      <c r="U61" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V61" s="6">
-        <v>0</v>
-      </c>
-      <c r="Z61" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA61" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:27" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="11" t="s">
+      <c r="U61" s="1"/>
+      <c r="V61" s="1"/>
+      <c r="X61" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y61" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z61" s="8"/>
+      <c r="AA61" s="9"/>
+      <c r="AG61" s="12"/>
+      <c r="AJ61" s="11">
+        <v>0</v>
+      </c>
+      <c r="AL61" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B62" s="1" t="s">
@@ -4622,15 +4799,18 @@
       <c r="R62">
         <v>0</v>
       </c>
-      <c r="U62" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V62" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:27" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="11" t="s">
+      <c r="U62" s="1"/>
+      <c r="V62" s="1"/>
+      <c r="X62" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y62" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG62" s="12"/>
+    </row>
+    <row r="63" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B63" s="1" t="s">
@@ -4678,15 +4858,18 @@
       <c r="R63">
         <v>0</v>
       </c>
-      <c r="U63" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V63" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:27" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="11" t="s">
+      <c r="U63" s="1"/>
+      <c r="V63" s="1"/>
+      <c r="X63" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y63" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG63" s="12"/>
+    </row>
+    <row r="64" spans="1:38" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -4734,15 +4917,18 @@
       <c r="R64">
         <v>0</v>
       </c>
-      <c r="U64" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V64" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A65" s="11" t="s">
+      <c r="U64" s="1"/>
+      <c r="V64" s="1"/>
+      <c r="X64" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y64" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG64" s="12"/>
+    </row>
+    <row r="65" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B65" s="1" t="s">
@@ -4790,15 +4976,18 @@
       <c r="R65">
         <v>0</v>
       </c>
-      <c r="U65" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V65" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:22" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="11" t="s">
+      <c r="U65" s="1"/>
+      <c r="V65" s="1"/>
+      <c r="X65" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y65" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG65" s="12"/>
+    </row>
+    <row r="66" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B66" s="1" t="s">
@@ -4846,15 +5035,18 @@
       <c r="R66">
         <v>1</v>
       </c>
-      <c r="U66" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V66" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:22" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="11" t="s">
+      <c r="U66" s="1"/>
+      <c r="V66" s="1"/>
+      <c r="X66" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y66" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG66" s="12"/>
+    </row>
+    <row r="67" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B67" s="1" t="s">
@@ -4902,15 +5094,18 @@
       <c r="R67">
         <v>1</v>
       </c>
-      <c r="U67" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V67" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:22" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="11" t="s">
+      <c r="U67" s="1"/>
+      <c r="V67" s="1"/>
+      <c r="X67" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y67" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG67" s="12"/>
+    </row>
+    <row r="68" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B68" s="1" t="s">
@@ -4958,15 +5153,18 @@
       <c r="R68">
         <v>0</v>
       </c>
-      <c r="U68" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V68" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A69" s="11" t="s">
+      <c r="U68" s="1"/>
+      <c r="V68" s="1"/>
+      <c r="X68" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y68" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG68" s="12"/>
+    </row>
+    <row r="69" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -5014,15 +5212,18 @@
       <c r="R69">
         <v>1</v>
       </c>
-      <c r="U69" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V69" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:22" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="11" t="s">
+      <c r="U69" s="1"/>
+      <c r="V69" s="1"/>
+      <c r="X69" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y69" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG69" s="12"/>
+    </row>
+    <row r="70" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B70" s="1" t="s">
@@ -5070,15 +5271,18 @@
       <c r="R70">
         <v>1</v>
       </c>
-      <c r="U70" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V70" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:22" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="11" t="s">
+      <c r="U70" s="1"/>
+      <c r="V70" s="1"/>
+      <c r="X70" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y70" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG70" s="12"/>
+    </row>
+    <row r="71" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B71" s="1" t="s">
@@ -5126,15 +5330,18 @@
       <c r="R71">
         <v>1</v>
       </c>
-      <c r="U71" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V71" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:22" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="11" t="s">
+      <c r="U71" s="1"/>
+      <c r="V71" s="1"/>
+      <c r="X71" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y71" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG71" s="12"/>
+    </row>
+    <row r="72" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B72" s="1" t="s">
@@ -5182,15 +5389,18 @@
       <c r="R72">
         <v>1</v>
       </c>
-      <c r="U72" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V72" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A73" s="11" t="s">
+      <c r="U72" s="1"/>
+      <c r="V72" s="1"/>
+      <c r="X72" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y72" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG72" s="12"/>
+    </row>
+    <row r="73" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B73" s="1" t="s">
@@ -5238,15 +5448,18 @@
       <c r="R73">
         <v>1</v>
       </c>
-      <c r="U73" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V73" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A74" s="11" t="s">
+      <c r="U73" s="1"/>
+      <c r="V73" s="1"/>
+      <c r="X73" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y73" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG73" s="12"/>
+    </row>
+    <row r="74" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B74" s="1" t="s">
@@ -5294,15 +5507,18 @@
       <c r="R74" s="4">
         <v>0</v>
       </c>
-      <c r="U74" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V74" s="6">
+      <c r="U74" s="1"/>
+      <c r="V74" s="1"/>
+      <c r="X74" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y74" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="75" spans="1:22" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="11" t="s">
+      <c r="AG74" s="12"/>
+    </row>
+    <row r="75" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B75" s="1" t="s">
@@ -5350,15 +5566,18 @@
       <c r="R75">
         <v>1</v>
       </c>
-      <c r="U75" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V75" s="6">
+      <c r="U75" s="1"/>
+      <c r="V75" s="1"/>
+      <c r="X75" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y75" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="76" spans="1:22" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="11" t="s">
+      <c r="AG75" s="12"/>
+    </row>
+    <row r="76" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B76" s="1" t="s">
@@ -5406,15 +5625,18 @@
       <c r="R76">
         <v>1</v>
       </c>
-      <c r="U76" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V76" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:22" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="11" t="s">
+      <c r="U76" s="1"/>
+      <c r="V76" s="1"/>
+      <c r="X76" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y76" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG76" s="12"/>
+    </row>
+    <row r="77" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B77" s="1" t="s">
@@ -5462,15 +5684,18 @@
       <c r="R77">
         <v>1</v>
       </c>
-      <c r="U77" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V77" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:22" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="11" t="s">
+      <c r="U77" s="1"/>
+      <c r="V77" s="1"/>
+      <c r="X77" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y77" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG77" s="12"/>
+    </row>
+    <row r="78" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B78" s="1" t="s">
@@ -5518,15 +5743,18 @@
       <c r="R78">
         <v>0</v>
       </c>
-      <c r="U78" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V78" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:22" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="11" t="s">
+      <c r="U78" s="1"/>
+      <c r="V78" s="1"/>
+      <c r="X78" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y78" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG78" s="12"/>
+    </row>
+    <row r="79" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B79" s="1" t="s">
@@ -5574,15 +5802,18 @@
       <c r="R79">
         <v>0</v>
       </c>
-      <c r="U79" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V79" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A80" s="11" t="s">
+      <c r="U79" s="1"/>
+      <c r="V79" s="1"/>
+      <c r="X79" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y79" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG79" s="12"/>
+    </row>
+    <row r="80" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B80" s="1" t="s">
@@ -5630,15 +5861,18 @@
       <c r="R80">
         <v>1</v>
       </c>
-      <c r="U80" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V80" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:22" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="11" t="s">
+      <c r="U80" s="1"/>
+      <c r="V80" s="1"/>
+      <c r="X80" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y80" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG80" s="12"/>
+    </row>
+    <row r="81" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B81" s="1" t="s">
@@ -5686,15 +5920,18 @@
       <c r="R81">
         <v>1</v>
       </c>
-      <c r="U81" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V81" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:22" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="11" t="s">
+      <c r="U81" s="1"/>
+      <c r="V81" s="1"/>
+      <c r="X81" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y81" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG81" s="12"/>
+    </row>
+    <row r="82" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B82" s="1" t="s">
@@ -5742,15 +5979,18 @@
       <c r="R82">
         <v>0</v>
       </c>
-      <c r="U82" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V82" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:22" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="11" t="s">
+      <c r="U82" s="1"/>
+      <c r="V82" s="1"/>
+      <c r="X82" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y82" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG82" s="12"/>
+    </row>
+    <row r="83" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B83" s="1" t="s">
@@ -5798,15 +6038,18 @@
       <c r="R83">
         <v>1</v>
       </c>
-      <c r="U83" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V83" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:22" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="11" t="s">
+      <c r="U83" s="1"/>
+      <c r="V83" s="1"/>
+      <c r="X83" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y83" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG83" s="12"/>
+    </row>
+    <row r="84" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B84" s="1" t="s">
@@ -5854,15 +6097,18 @@
       <c r="R84">
         <v>1</v>
       </c>
-      <c r="U84" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V84" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:22" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="11" t="s">
+      <c r="U84" s="1"/>
+      <c r="V84" s="1"/>
+      <c r="X84" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y84" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG84" s="12"/>
+    </row>
+    <row r="85" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B85" s="1" t="s">
@@ -5910,15 +6156,18 @@
       <c r="R85">
         <v>0</v>
       </c>
-      <c r="U85" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V85" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A86" s="11" t="s">
+      <c r="U85" s="1"/>
+      <c r="V85" s="1"/>
+      <c r="X85" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y85" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG85" s="12"/>
+    </row>
+    <row r="86" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B86" s="1" t="s">
@@ -5966,15 +6215,18 @@
       <c r="R86">
         <v>0</v>
       </c>
-      <c r="U86" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V86" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:22" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="11" t="s">
+      <c r="U86" s="1"/>
+      <c r="V86" s="1"/>
+      <c r="X86" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y86" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG86" s="12"/>
+    </row>
+    <row r="87" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B87" s="1" t="s">
@@ -6022,15 +6274,18 @@
       <c r="R87">
         <v>1</v>
       </c>
-      <c r="U87" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V87" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:22" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="11" t="s">
+      <c r="U87" s="1"/>
+      <c r="V87" s="1"/>
+      <c r="X87" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y87" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG87" s="12"/>
+    </row>
+    <row r="88" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B88" s="1" t="s">
@@ -6078,15 +6333,18 @@
       <c r="R88">
         <v>1</v>
       </c>
-      <c r="U88" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V88" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A89" s="11" t="s">
+      <c r="U88" s="1"/>
+      <c r="V88" s="1"/>
+      <c r="X88" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y88" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG88" s="12"/>
+    </row>
+    <row r="89" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B89" s="1" t="s">
@@ -6134,15 +6392,18 @@
       <c r="R89">
         <v>0</v>
       </c>
-      <c r="U89" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V89" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:22" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="11" t="s">
+      <c r="U89" s="1"/>
+      <c r="V89" s="1"/>
+      <c r="X89" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y89" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG89" s="12"/>
+    </row>
+    <row r="90" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B90" s="1" t="s">
@@ -6190,15 +6451,18 @@
       <c r="R90">
         <v>1</v>
       </c>
-      <c r="U90" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V90" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:22" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="11" t="s">
+      <c r="U90" s="1"/>
+      <c r="V90" s="1"/>
+      <c r="X90" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y90" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG90" s="12"/>
+    </row>
+    <row r="91" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B91" s="1" t="s">
@@ -6246,15 +6510,18 @@
       <c r="R91">
         <v>0</v>
       </c>
-      <c r="U91" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V91" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:22" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="11" t="s">
+      <c r="U91" s="1"/>
+      <c r="V91" s="1"/>
+      <c r="X91" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y91" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG91" s="12"/>
+    </row>
+    <row r="92" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B92" s="1" t="s">
@@ -6302,15 +6569,18 @@
       <c r="R92">
         <v>0</v>
       </c>
-      <c r="U92" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V92" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A93" s="11" t="s">
+      <c r="U92" s="1"/>
+      <c r="V92" s="1"/>
+      <c r="X92" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y92" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG92" s="12"/>
+    </row>
+    <row r="93" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B93" s="1" t="s">
@@ -6358,15 +6628,18 @@
       <c r="R93">
         <v>0</v>
       </c>
-      <c r="U93" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V93" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A94" s="11" t="s">
+      <c r="U93" s="1"/>
+      <c r="V93" s="1"/>
+      <c r="X93" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y93" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG93" s="12"/>
+    </row>
+    <row r="94" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B94" s="1" t="s">
@@ -6414,15 +6687,18 @@
       <c r="R94">
         <v>0</v>
       </c>
-      <c r="U94" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V94" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:22" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="11" t="s">
+      <c r="U94" s="1"/>
+      <c r="V94" s="1"/>
+      <c r="X94" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y94" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG94" s="12"/>
+    </row>
+    <row r="95" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B95" s="1" t="s">
@@ -6470,15 +6746,18 @@
       <c r="R95">
         <v>0</v>
       </c>
-      <c r="U95" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="V95" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A96" s="11" t="s">
+      <c r="U95" s="1"/>
+      <c r="V95" s="1"/>
+      <c r="X95" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y95" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG95" s="12"/>
+    </row>
+    <row r="96" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B96" s="1" t="s">
@@ -6526,15 +6805,18 @@
       <c r="R96">
         <v>1</v>
       </c>
-      <c r="U96" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V96" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A97" s="11" t="s">
+      <c r="U96" s="1"/>
+      <c r="V96" s="1"/>
+      <c r="X96" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y96" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG96" s="12"/>
+    </row>
+    <row r="97" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B97" s="1" t="s">
@@ -6582,12 +6864,15 @@
       <c r="R97">
         <v>1</v>
       </c>
-      <c r="U97" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="V97" s="6">
-        <v>1</v>
-      </c>
+      <c r="U97" s="1"/>
+      <c r="V97" s="1"/>
+      <c r="X97" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y97" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG97" s="12"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -6600,11 +6885,517 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4424583A-B452-4D7A-A8D1-0A2BFAF53B6C}">
+  <dimension ref="A1:B61"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>0</v>
+      </c>
+      <c r="B3" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>0</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>0</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>0</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>2</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>0</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>0</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>0</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>0</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>0</v>
+      </c>
+      <c r="B12" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>1</v>
+      </c>
+      <c r="B13" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>0</v>
+      </c>
+      <c r="B14" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>2</v>
+      </c>
+      <c r="B15" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>0</v>
+      </c>
+      <c r="B16" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>0</v>
+      </c>
+      <c r="B17" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>1</v>
+      </c>
+      <c r="B18" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>5</v>
+      </c>
+      <c r="B19" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>0</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>0</v>
+      </c>
+      <c r="B21" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>0</v>
+      </c>
+      <c r="B22" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>0</v>
+      </c>
+      <c r="B23" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>0</v>
+      </c>
+      <c r="B24" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>0</v>
+      </c>
+      <c r="B25" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>0</v>
+      </c>
+      <c r="B26" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>1</v>
+      </c>
+      <c r="B27" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="6">
+        <v>0</v>
+      </c>
+      <c r="B28" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>0</v>
+      </c>
+      <c r="B29" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>3</v>
+      </c>
+      <c r="B30" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>1</v>
+      </c>
+      <c r="B31" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <v>2</v>
+      </c>
+      <c r="B32" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="6">
+        <v>0</v>
+      </c>
+      <c r="B33" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
+        <v>0</v>
+      </c>
+      <c r="B34" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="6">
+        <v>0</v>
+      </c>
+      <c r="B35" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="6">
+        <v>0</v>
+      </c>
+      <c r="B36" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="6">
+        <v>0</v>
+      </c>
+      <c r="B37" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="6">
+        <v>0</v>
+      </c>
+      <c r="B38">
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="6">
+        <v>0</v>
+      </c>
+      <c r="B39">
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="6">
+        <v>0</v>
+      </c>
+      <c r="B40">
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="6">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="6">
+        <v>0</v>
+      </c>
+      <c r="B42">
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="6">
+        <v>0</v>
+      </c>
+      <c r="B43">
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="6">
+        <v>1</v>
+      </c>
+      <c r="B44">
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="6">
+        <v>0</v>
+      </c>
+      <c r="B45">
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="6">
+        <v>2</v>
+      </c>
+      <c r="B46">
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="6">
+        <v>0</v>
+      </c>
+      <c r="B47">
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="6">
+        <v>0</v>
+      </c>
+      <c r="B48">
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="6">
+        <v>0</v>
+      </c>
+      <c r="B49">
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="6">
+        <v>0</v>
+      </c>
+      <c r="B50">
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="6">
+        <v>0</v>
+      </c>
+      <c r="B51">
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="6">
+        <v>0</v>
+      </c>
+      <c r="B52">
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="6">
+        <v>1</v>
+      </c>
+      <c r="B53">
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="6">
+        <v>0</v>
+      </c>
+      <c r="B54">
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="6">
+        <v>0</v>
+      </c>
+      <c r="B55">
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="6">
+        <v>0</v>
+      </c>
+      <c r="B56">
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="6">
+        <v>0</v>
+      </c>
+      <c r="B57">
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="6">
+        <v>0</v>
+      </c>
+      <c r="B58">
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="6">
+        <v>0</v>
+      </c>
+      <c r="B59">
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="6">
+        <v>0</v>
+      </c>
+      <c r="B60">
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="6">
+        <v>0</v>
+      </c>
+      <c r="B61">
+        <v>0.61111111111111116</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57693BD7-5CAC-4E0F-9C9F-5AF7BC842981}">
   <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>